<commit_message>
black border to images Refactor worksheet selection change event handling and image highlighting
</commit_message>
<xml_diff>
--- a/save.xlsx
+++ b/save.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\health\news_underground\mediaSorter\programs\excel_prog\mediaSorter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F253971B-75A5-49E7-9EEE-3092EED1B1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF6D08D-1DB1-4585-8FEA-347ABB48E834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{0347F06F-BF31-4DAA-A040-06373AA40A3E}"/>
   </bookViews>
@@ -402,9 +402,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6707F55-20AE-4723-B093-FEE1EC6B56F1}">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>